<commit_message>
textos melhorados e adicionado sinalizacao no rastrear
</commit_message>
<xml_diff>
--- a/Traduzido/PTBR/Lang/PTBR/Game/Element.xlsx
+++ b/Traduzido/PTBR/Lang/PTBR/Game/Element.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7181415-1116-4601-A3DF-D86FCF2CE002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C147C68-5775-4BF9-8020-26A25E00891F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3060" windowWidth="17790" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Element" sheetId="1" r:id="rId1"/>
@@ -25962,12 +25962,15 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V1" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="C231" sqref="C231"/>
+      <selection pane="bottomLeft" activeCell="F224" sqref="F224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="5" width="16" customWidth="1"/>
+    <col min="1" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="247.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="16" customWidth="1"/>
     <col min="12" max="12" width="52.5703125" bestFit="1" customWidth="1"/>

</xml_diff>